<commit_message>
prese misure a distanza fissa
</commit_message>
<xml_diff>
--- a/BILANCIA DI COLUMB/CSV/bilancia di columb dati.xlsx
+++ b/BILANCIA DI COLUMB/CSV/bilancia di columb dati.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="misure iniziali" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="6kV" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="d=10cm cambio volt" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">diametro sfere</t>
   </si>
@@ -41,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">teta AVG</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -661,7 +665,7 @@
         <v>186</v>
       </c>
       <c r="E2" s="2">
-        <f>AVERAGE(B2:D2)</f>
+        <f t="shared" ref="E2:E8" si="0">AVERAGE(B2:D2)</f>
         <v>186.33333333333334</v>
       </c>
     </row>
@@ -679,7 +683,7 @@
         <v>126</v>
       </c>
       <c r="E3" s="2">
-        <f>AVERAGE(B3:D3)</f>
+        <f t="shared" si="0"/>
         <v>124.66666666666667</v>
       </c>
     </row>
@@ -697,7 +701,7 @@
         <v>103</v>
       </c>
       <c r="E4" s="2">
-        <f>AVERAGE(B4:D4)</f>
+        <f t="shared" si="0"/>
         <v>105.33333333333333</v>
       </c>
     </row>
@@ -715,7 +719,7 @@
         <v>90</v>
       </c>
       <c r="E5" s="2">
-        <f>AVERAGE(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>92.333333333333329</v>
       </c>
     </row>
@@ -733,7 +737,7 @@
         <v>51</v>
       </c>
       <c r="E6" s="2">
-        <f>AVERAGE(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
@@ -751,7 +755,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="2">
-        <f>AVERAGE(B7:D7)</f>
+        <f t="shared" si="0"/>
         <v>32.333333333333336</v>
       </c>
     </row>
@@ -769,7 +773,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="2">
-        <f>AVERAGE(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -936,6 +940,108 @@
     <row r="48" ht="14.25">
       <c r="B48" s="2"/>
     </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+      <c r="C5">
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>72</v>
+      </c>
+      <c r="D6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>